<commit_message>
Saya edit backend tabel destinasi dan pengguna
</commit_message>
<xml_diff>
--- a/assets/excel/Data dokter.xlsx
+++ b/assets/excel/Data dokter.xlsx
@@ -15,42 +15,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
   <si>
     <t>ID</t>
   </si>
   <si>
-    <t>Nama Obat</t>
-  </si>
-  <si>
-    <t>Spesialis</t>
-  </si>
-  <si>
-    <t>Alamat</t>
-  </si>
-  <si>
-    <t>No Telpon</t>
-  </si>
-  <si>
-    <t>Spesialis Penyakit Dalam</t>
-  </si>
-  <si>
-    <t>Bantul, Yogyakarta</t>
-  </si>
-  <si>
-    <t>Spesialis Gigi</t>
-  </si>
-  <si>
-    <t>KulonProgo, Yogyakarta</t>
-  </si>
-  <si>
-    <t>Spesialis Anak</t>
-  </si>
-  <si>
-    <t>Sleman, Yogyakarta</t>
-  </si>
-  <si>
-    <t>Spesialis Mata</t>
+    <t>Nama Pengguna</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Tanggal Lahir</t>
+  </si>
+  <si>
+    <t>Arslan Wiratama</t>
+  </si>
+  <si>
+    <t>d41d8cd98f00b204e9800998ecf8427e</t>
+  </si>
+  <si>
+    <t>izzuddinalfatah33@gmail.com</t>
+  </si>
+  <si>
+    <t>2003-04-07</t>
+  </si>
+  <si>
+    <t>Yusril Camelia</t>
+  </si>
+  <si>
+    <t>izzalfatah347@gmail.com</t>
+  </si>
+  <si>
+    <t>2004-09-22</t>
+  </si>
+  <si>
+    <t>Ravin Sadewa</t>
+  </si>
+  <si>
+    <t>muhalfatah743@gmail.com</t>
+  </si>
+  <si>
+    <t>2005-01-11</t>
   </si>
 </sst>
 </file>
@@ -389,7 +398,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -416,58 +425,53 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2">
-        <v>12211882</v>
-      </c>
-      <c r="B2">
-        <v>85677914566</v>
+        <v>12211845</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3">
-        <v>12211883</v>
-      </c>
-      <c r="B3">
-        <v>87566431104</v>
+        <v>12211846</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4">
-        <v>12211884</v>
-      </c>
-      <c r="B4">
-        <v>856335700231</v>
+        <v>12211847</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5">
-        <v>12211885</v>
-      </c>
-      <c r="B5">
-        <v>87843557324</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>